<commit_message>
loging, auto-correlation is not there. combining ac1/hc1 might be good
</commit_message>
<xml_diff>
--- a/Progress-notes/tools.xlsx
+++ b/Progress-notes/tools.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="4245" yWindow="750" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -381,7 +381,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -418,24 +418,24 @@
         <v>16000</v>
       </c>
       <c r="C2">
-        <f>$A2/(24*60)</f>
-        <v>11.111111111111111</v>
+        <f>$A2*7/5/(24*60)</f>
+        <v>15.555555555555555</v>
       </c>
       <c r="D2">
-        <f>$A2/(24*60/5)</f>
-        <v>55.555555555555557</v>
+        <f>$A2*7/5/(24*60/5)</f>
+        <v>77.777777777777771</v>
       </c>
       <c r="E2">
-        <f>$A2/(24*60/15)</f>
-        <v>166.66666666666666</v>
+        <f>$A2*7/5/(24*60/15)</f>
+        <v>233.33333333333334</v>
       </c>
       <c r="F2">
-        <f>$A2/(24*60/30)</f>
-        <v>333.33333333333331</v>
+        <f>$A2*7/5/(24*60/30)</f>
+        <v>466.66666666666669</v>
       </c>
       <c r="G2">
-        <f>$A2/(24)</f>
-        <v>666.66666666666663</v>
+        <f>$A2*7/5/(24)</f>
+        <v>933.33333333333337</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -444,23 +444,23 @@
       </c>
       <c r="C3">
         <f>C2/30</f>
-        <v>0.37037037037037035</v>
+        <v>0.51851851851851849</v>
       </c>
       <c r="D3">
         <f t="shared" ref="D3:G3" si="0">D2/30</f>
-        <v>1.8518518518518519</v>
+        <v>2.5925925925925926</v>
       </c>
       <c r="E3">
         <f t="shared" si="0"/>
-        <v>5.5555555555555554</v>
+        <v>7.7777777777777777</v>
       </c>
       <c r="F3">
         <f t="shared" si="0"/>
-        <v>11.111111111111111</v>
+        <v>15.555555555555555</v>
       </c>
       <c r="G3">
         <f t="shared" si="0"/>
-        <v>22.222222222222221</v>
+        <v>31.111111111111111</v>
       </c>
     </row>
   </sheetData>

</xml_diff>